<commit_message>
Added Nifty transistions to the powerpoint presentation
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -102,17 +102,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="2400" baseline="0"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Strassen</a:t>
+              <a:rPr lang="en-US" sz="2400" baseline="0"/>
+              <a:t>Strassen algorithm vs Triple loop</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> algorithm vs Triple loop</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -744,11 +739,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="90949504"/>
-        <c:axId val="90947968"/>
+        <c:axId val="73336704"/>
+        <c:axId val="73351168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90949504"/>
+        <c:axId val="73336704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -761,10 +756,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000" baseline="0"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
                   <a:t>N - matrix size</a:t>
                 </a:r>
               </a:p>
@@ -777,12 +772,22 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90947968"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" baseline="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="73351168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90947968"/>
+        <c:axId val="73351168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -796,10 +801,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000" baseline="0"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
                   <a:t>Time taken (s)</a:t>
                 </a:r>
               </a:p>
@@ -812,7 +817,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90949504"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" baseline="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="73336704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -821,6 +836,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" baseline="0"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -855,10 +880,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="2400" baseline="0"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2400" baseline="0"/>
               <a:t>4 Threads</a:t>
             </a:r>
           </a:p>
@@ -1017,11 +1042,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="87450752"/>
-        <c:axId val="87442944"/>
+        <c:axId val="73389952"/>
+        <c:axId val="74383360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87450752"/>
+        <c:axId val="73389952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1034,10 +1059,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000" baseline="0"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
                   <a:t>N - matrix size</a:t>
                 </a:r>
               </a:p>
@@ -1050,12 +1075,22 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87442944"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" baseline="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="74383360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87442944"/>
+        <c:axId val="74383360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,10 +1104,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000" baseline="0"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
                   <a:t>Time taken (s)</a:t>
                 </a:r>
               </a:p>
@@ -1085,7 +1120,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87450752"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" baseline="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="73389952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1094,6 +1139,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" baseline="0"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1128,10 +1183,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="2400" baseline="0"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2400" baseline="0"/>
               <a:t>1 Thread</a:t>
             </a:r>
           </a:p>
@@ -1290,11 +1345,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="93686016"/>
-        <c:axId val="93684480"/>
+        <c:axId val="74422144"/>
+        <c:axId val="74424320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93686016"/>
+        <c:axId val="74422144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1307,10 +1362,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000" baseline="0"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
                   <a:t>N - matrix size</a:t>
                 </a:r>
               </a:p>
@@ -1323,12 +1378,22 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93684480"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" baseline="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="74424320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93684480"/>
+        <c:axId val="74424320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1342,10 +1407,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000" baseline="0"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
                   <a:t>Time Taken (s)</a:t>
                 </a:r>
               </a:p>
@@ -1358,7 +1423,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93686016"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" baseline="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="74422144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1367,6 +1442,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" baseline="0"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1385,15 +1470,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>581024</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>647699</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1414,16 +1499,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1444,16 +1529,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1825,8 +1910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated stuff with the OpenMPI data.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9114"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="293"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="293" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Plots" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Strassen</t>
   </si>
@@ -25,6 +25,9 @@
   </si>
   <si>
     <t>Regular</t>
+  </si>
+  <si>
+    <t>OpenMPI</t>
   </si>
 </sst>
 </file>
@@ -106,7 +109,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2400" baseline="0"/>
-              <a:t>Strassen algorithm vs Triple loop</a:t>
+              <a:t>OpenMP Strassen</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -135,7 +138,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$H$2</c:f>
+              <c:f>Data!$B$2:$H$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -165,7 +168,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$H$6</c:f>
+              <c:f>Data!$B$6:$H$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -210,7 +213,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$H$2</c:f>
+              <c:f>Data!$B$2:$H$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -240,7 +243,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$H$5</c:f>
+              <c:f>Data!$B$5:$H$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -285,7 +288,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$H$2</c:f>
+              <c:f>Data!$B$2:$H$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -315,7 +318,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$H$4</c:f>
+              <c:f>Data!$B$4:$H$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -360,7 +363,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$H$2</c:f>
+              <c:f>Data!$B$2:$H$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -390,7 +393,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$H$3</c:f>
+              <c:f>Data!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -414,317 +417,6 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>638.63927899999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:v>Regular 1t</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$9:$H$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4096</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$10:$H$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>4.058E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7877999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.14174499999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2158929999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11.172612000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>105.337958</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1084.4397120000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:v>Regular 2t</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:spPr>
-              <a:ln cmpd="sng">
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$9:$H$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4096</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$11:$H$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>2.052E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.4022999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.5482999999999995E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.62887399999999993</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.6212679999999997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>55.299827999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>578.07848200000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:v>Regular 3t</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$9:$H$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4096</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$12:$H$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.4349999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.1018E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.9995999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.42952299999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.6760539999999997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>36.570000999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>384.28114199999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:v>Regular 4t</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C00000" mc:Ignorable=""/>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$9:$H$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4096</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$13:$H$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.0449999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.899999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.7266000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.31682699999999997</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.764364</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>27.990532000000002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>304.08810699999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -739,11 +431,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="73336704"/>
-        <c:axId val="73351168"/>
+        <c:axId val="93813760"/>
+        <c:axId val="93815936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73336704"/>
+        <c:axId val="93813760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -782,12 +474,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73351168"/>
+        <c:crossAx val="93815936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73351168"/>
+        <c:axId val="93815936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -827,7 +519,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73336704"/>
+        <c:crossAx val="93813760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -853,7 +545,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -899,14 +591,14 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Strassen 4t</c:v>
+            <c:v>Regular 4t</c:v>
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$H$2</c:f>
+              <c:f>Data!$B$9:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -936,30 +628,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$H$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>2.9020000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.9668999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.8347999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.32338499999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.1996790000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15.210084</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>182.46132600000001</c:v>
+              <c:f>Data!$B$13:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0449999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.899999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7266000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.31682699999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.764364</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.990532000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>304.08810699999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -967,14 +659,14 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Regular 4t</c:v>
+            <c:v>OpenMP 4t</c:v>
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$H$9</c:f>
+              <c:f>Data!$B$2:$H$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1004,30 +696,98 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$H$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.0449999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.899999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.7266000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.31682699999999997</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.764364</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>27.990532000000002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>304.08810699999998</c:v>
+              <c:f>Data!$B$6:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.9020000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9668999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8347999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.32338499999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1996790000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.210084</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>182.46132600000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>MPI 4t</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$B$16:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$B$20:$H$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.4344000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0837E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.142788</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.403833</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4750000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.1274670000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.339838999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1042,13 +802,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="73389952"/>
-        <c:axId val="74383360"/>
+        <c:axId val="93834240"/>
+        <c:axId val="93840512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73389952"/>
+        <c:axId val="93834240"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:min val="50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1085,14 +847,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74383360"/>
+        <c:crossAx val="93840512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74383360"/>
+        <c:axId val="93840512"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:max val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1130,7 +894,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73389952"/>
+        <c:crossAx val="93834240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1156,7 +920,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1202,14 +966,14 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Strassen 1t</c:v>
+            <c:v>Regular 1t</c:v>
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$H$2</c:f>
+              <c:f>Data!$B$9:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1239,30 +1003,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$H$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>4.6309999999999997E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.7961999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.15857599999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.049974</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.7579570000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>55.477885000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>638.63927899999999</c:v>
+              <c:f>Data!$B$10:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.058E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7877999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14174499999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2158929999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.172612000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>105.337958</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1084.4397120000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1270,14 +1034,14 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Regular 1t</c:v>
+            <c:v>OpenMP 1t</c:v>
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$H$9</c:f>
+              <c:f>Data!$B$2:$H$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1307,30 +1071,98 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$H$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>4.058E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7877999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.14174499999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2158929999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11.172612000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>105.337958</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1084.4397120000001</c:v>
+              <c:f>Data!$B$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.6309999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7961999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15857599999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.049974</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.7579570000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>55.477885000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>638.63927899999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>MPI 1t</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$B$16:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$B$17:$H$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.2874999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0834999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14274899999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.492506</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1993309999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.340468</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>93.290227000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1345,11 +1177,453 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="74422144"/>
-        <c:axId val="74424320"/>
+        <c:axId val="103058432"/>
+        <c:axId val="103064704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74422144"/>
+        <c:axId val="103058432"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" baseline="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                  <a:t>N - matrix size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" baseline="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="103064704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="103064704"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" baseline="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                  <a:t>Time Taken (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" baseline="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="103058432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" baseline="0"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" baseline="0"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" baseline="0"/>
+              <a:t>MPI Implementation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>MPI 1t</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$B$16:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$B$17:$H$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.2874999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0834999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14274899999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.492506</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1993309999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.340468</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>93.290227000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>MPI 2t</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$B$16:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$B$18:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.3939E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.1205000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14205000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.43188700000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7896920000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.8760639999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>87.929826000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>MPI 3t</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$B$16:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$B$19:$H$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.453E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0937000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14303399999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.41612300000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5722640000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.3049200000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50.195720000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>MPI 4t</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$B$16:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$B$20:$H$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.4344000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0837E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.142788</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.403833</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4750000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.1274670000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.339838999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="91767168"/>
+        <c:axId val="91769088"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="91767168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1388,12 +1662,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74424320"/>
+        <c:crossAx val="91769088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74424320"/>
+        <c:axId val="91769088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1433,7 +1707,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74422144"/>
+        <c:crossAx val="91767168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1465,24 +1739,491 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" baseline="0"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" baseline="0"/>
+              <a:t>Regular Multiplication w/ openMP</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Regular 4t</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C00000" mc:Ignorable=""/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$B$2:$H$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$B$13:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0449999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.899999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7266000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.31682699999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.764364</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.990532000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>304.08810699999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Regular 3t</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$B$2:$H$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$B$12:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.4349999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1018E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9995999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42952299999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6760539999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36.570000999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>384.28114199999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Regular 2t</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$B$2:$H$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$B$11:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.052E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4022999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.5482999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.62887399999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.6212679999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>55.299827999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>578.07848200000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Regular 1t</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$B$2:$H$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$B$10:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.058E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7877999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14174499999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2158929999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.172612000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>105.337958</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1084.4397120000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="95139328"/>
+        <c:axId val="95141248"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="95139328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" baseline="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                  <a:t>N - matrix size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" baseline="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="95141248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="95141248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" baseline="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                  <a:t>Time taken (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" baseline="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="95139328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" baseline="0"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>66674</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:colOff>493060</xdr:colOff>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1500,19 +2241,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>161924</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>131668</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>533399</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:colOff>483534</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>131668</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1530,19 +2271,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>160804</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:colOff>474010</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>141754</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="7" name="Chart 6"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1552,6 +2293,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>19048</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>493060</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1908,10 +2713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1946,9 +2751,7 @@
       <c r="H2" s="1">
         <v>4096</v>
       </c>
-      <c r="I2" s="1">
-        <v>8192</v>
-      </c>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -2092,9 +2895,7 @@
       <c r="H9" s="1">
         <v>4096</v>
       </c>
-      <c r="I9" s="1">
-        <v>8192</v>
-      </c>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -2200,14 +3001,149 @@
         <v>304.08810699999998</v>
       </c>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <v>64</v>
+      </c>
+      <c r="C16" s="1">
+        <v>128</v>
+      </c>
+      <c r="D16" s="1">
+        <v>256</v>
+      </c>
+      <c r="E16" s="1">
+        <v>512</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1024</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2048</v>
+      </c>
+      <c r="H16" s="1">
+        <v>4096</v>
+      </c>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>1.2874999999999999E-2</v>
+      </c>
+      <c r="C17">
+        <v>5.0834999999999998E-2</v>
+      </c>
+      <c r="D17">
+        <v>0.14274899999999999</v>
+      </c>
+      <c r="E17">
+        <v>0.492506</v>
+      </c>
+      <c r="F17">
+        <v>2.1993309999999999</v>
+      </c>
+      <c r="G17">
+        <v>12.340468</v>
+      </c>
+      <c r="H17">
+        <v>93.290227000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>1.3939E-2</v>
+      </c>
+      <c r="C18">
+        <v>5.1205000000000001E-2</v>
+      </c>
+      <c r="D18">
+        <v>0.14205000000000001</v>
+      </c>
+      <c r="E18">
+        <v>0.43188700000000002</v>
+      </c>
+      <c r="F18">
+        <v>1.7896920000000001</v>
+      </c>
+      <c r="G18">
+        <v>9.8760639999999995</v>
+      </c>
+      <c r="H18">
+        <v>87.929826000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>1.453E-2</v>
+      </c>
+      <c r="C19">
+        <v>5.0937000000000003E-2</v>
+      </c>
+      <c r="D19">
+        <v>0.14303399999999999</v>
+      </c>
+      <c r="E19">
+        <v>0.41612300000000002</v>
+      </c>
+      <c r="F19">
+        <v>1.5722640000000001</v>
+      </c>
+      <c r="G19">
+        <v>7.3049200000000001</v>
+      </c>
+      <c r="H19">
+        <v>50.195720000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>1.4344000000000001E-2</v>
+      </c>
+      <c r="C20">
+        <v>5.0837E-2</v>
+      </c>
+      <c r="D20">
+        <v>0.142788</v>
+      </c>
+      <c r="E20">
+        <v>0.403833</v>
+      </c>
+      <c r="F20">
+        <v>1.4750000000000001</v>
+      </c>
+      <c r="G20">
+        <v>7.1274670000000002</v>
+      </c>
+      <c r="H20">
+        <v>33.339838999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2215,7 +3151,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -2225,6 +3163,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>